<commit_message>
add 4 hour version
</commit_message>
<xml_diff>
--- a/src/source/table2.xlsx
+++ b/src/source/table2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowHeight="17680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>鸠江区三线水位测站记录情况登记表</t>
   </si>
@@ -44,15 +44,9 @@
     <t>三线水位</t>
   </si>
   <si>
-    <t>昨日8时</t>
-  </si>
-  <si>
     <t>两比</t>
   </si>
   <si>
-    <t>两小时内</t>
-  </si>
-  <si>
     <t>2020年最高水位</t>
   </si>
   <si>
@@ -65,8 +59,20 @@
     <t>发生时间</t>
   </si>
   <si>
-    <t>无为大堤：
-（测站：凤凰颈闸下）</t>
+    <r>
+      <t xml:space="preserve">无为大堤：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（测站：凤凰颈闸下）</t>
+    </r>
   </si>
   <si>
     <t>设防水位：11.5
@@ -128,8 +134,20 @@
 保证水位：11.5</t>
   </si>
   <si>
-    <t>惠生连圩堤：
-（测站：凤凰颈闸下）</t>
+    <r>
+      <t xml:space="preserve">惠生连圩堤：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（测站：凤凰颈闸下）</t>
+    </r>
   </si>
   <si>
     <t>设防水位：11.5
@@ -137,12 +155,36 @@
 保证水位：14.5</t>
   </si>
   <si>
-    <t>永定大圩堤：
-（测站：凤凰颈闸下）</t>
-  </si>
-  <si>
-    <t>黑沙洲、天然洲圩：
-（测站：凤凰颈闸下）</t>
+    <r>
+      <t xml:space="preserve">永定大圩堤：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（测站：凤凰颈闸下）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">黑沙洲、天然洲圩：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（测站：凤凰颈闸下）</t>
+    </r>
   </si>
   <si>
     <t>设防水位：11
@@ -151,7 +193,7 @@
   </si>
   <si>
     <t>备注：1、数据来源为查询安徽水信息网所得；
-     2、浅蓝色为超设防水位，深蓝色为超警戒水位，红色为超保证水位。</t>
+      2、浅蓝色为超设防水位，深蓝色为超警戒水位，红色为超保证水位。</t>
   </si>
   <si>
     <t/>
@@ -169,7 +211,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="\+0.00;\-0.00"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +244,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -790,137 +839,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="11">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="13">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="11">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="13">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -955,13 +1004,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -970,19 +1019,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -996,10 +1048,10 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1324,25 +1376,25 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="8" width="11.875" customWidth="1"/>
-    <col min="9" max="10" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="3.75454545454545" customWidth="1"/>
+    <col min="2" max="2" width="18.8181818181818" customWidth="1"/>
+    <col min="3" max="3" width="15.6272727272727" customWidth="1"/>
+    <col min="4" max="8" width="11.8727272727273" customWidth="1"/>
+    <col min="9" max="10" width="11.2545454545455" customWidth="1"/>
     <col min="11" max="16384" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="21" customHeight="1" spans="1:1">
+    <row r="1" s="1" customFormat="1" ht="24" customHeight="1" spans="1:1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="14.25" customHeight="1" spans="1:1">
+    <row r="2" customFormat="1" ht="20" customHeight="1" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1359,55 +1411,51 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="25"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" s="2" customFormat="1" ht="20" customHeight="1" spans="1:10">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="J4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="5" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="5" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A5" s="10">
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -1420,22 +1468,22 @@
         <f>D5-E5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="27">
         <v>44025</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="28">
         <v>15.21</v>
       </c>
     </row>
-    <row r="6" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="6" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A6" s="15">
         <v>2</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -1448,22 +1496,22 @@
         <f>D6-E6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="27">
         <v>44033</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="28">
         <v>12.76</v>
       </c>
     </row>
-    <row r="7" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="7" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A7" s="15">
         <v>3</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -1476,22 +1524,22 @@
         <f t="shared" ref="H7:H14" si="1">D7-E7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="27">
         <v>44033</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="29">
         <v>12.72</v>
       </c>
     </row>
-    <row r="8" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="8" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A8" s="15">
         <v>4</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -1504,22 +1552,22 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="27">
         <v>44029</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="28">
         <v>13.19</v>
       </c>
     </row>
-    <row r="9" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="9" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A9" s="15">
         <v>5</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -1532,26 +1580,26 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="27">
         <v>44033</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="29">
         <v>12.72</v>
       </c>
     </row>
-    <row r="10" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="10" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A10" s="15">
         <v>6</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>22</v>
+      <c r="B10" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+        <v>21</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1560,26 +1608,26 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="27">
         <v>44033</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="29">
         <v>12.77</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="11" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A11" s="15">
         <v>7</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+        <v>23</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1588,22 +1636,22 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="26">
+      <c r="I11" s="27">
         <v>44030</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="29">
         <v>12.1</v>
       </c>
     </row>
-    <row r="12" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="12" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A12" s="15">
         <v>8</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1616,22 +1664,22 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="27">
         <v>44025</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="29">
         <v>15.21</v>
       </c>
     </row>
-    <row r="13" s="3" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
+    <row r="13" s="3" customFormat="1" ht="40" customHeight="1" spans="1:10">
       <c r="A13" s="15">
         <v>9</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -1644,26 +1692,26 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I13" s="26">
+      <c r="I13" s="27">
         <v>44025</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="29">
         <v>15.21</v>
       </c>
     </row>
-    <row r="14" customFormat="1" ht="38.25" customHeight="1" spans="1:10">
-      <c r="A14" s="20">
+    <row r="14" customFormat="1" ht="40" customHeight="1" spans="1:10">
+      <c r="A14" s="21">
         <v>10</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+        <v>28</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1672,30 +1720,30 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="27">
         <v>44025</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="29">
         <v>15.21</v>
       </c>
     </row>
     <row r="15" customFormat="1" ht="34" customHeight="1" spans="1:10">
-      <c r="A15" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
+      <c r="A15" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16" customFormat="1" spans="1:1">
-      <c r="A16" s="24" t="s">
-        <v>32</v>
+      <c r="A16" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>